<commit_message>
Added parsing and checking data
Parsing through the excel sheet and storing values in variables
Checking validity of all data and output and informational message on error
</commit_message>
<xml_diff>
--- a/python/Order.xlsx
+++ b/python/Order.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisazaher/Documents/UNIVERSITY/4TH YR/ECE496 - Capstone/githubrepo/crapstone/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD69705E-C009-A94C-A48A-9DF00C2A1124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376F5AF4-9E36-6B4B-B73C-C6D04B51109F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="520" windowWidth="28040" windowHeight="15900" xr2:uid="{818555DF-D87D-7744-A63A-8FE4BECED375}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15840" xr2:uid="{818555DF-D87D-7744-A63A-8FE4BECED375}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -569,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08B7C6A-020E-CF41-9ABD-0299F7C7C68B}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,33 +609,41 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{FD75194D-5B9D-4846-B8FA-405AD3509F60}">
+      <formula1>1</formula1>
+      <formula2>2</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7E1FDA63-8451-0A4D-B352-83FFA0198F24}">
-          <x14:formula1>
-            <xm:f>Sheet2!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7622BCE3-22F7-064D-ACE8-3582754E0FF4}">
-          <x14:formula1>
-            <xm:f>Sheet2!$B:$B</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1778CEE5-16D4-C144-91D7-649D76D9D307}">
-          <x14:formula1>
-            <xm:f>Sheet2!$C:$C</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:H2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -643,7 +652,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B1" sqref="B1:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added encoding and serial communication
</commit_message>
<xml_diff>
--- a/python/Order.xlsx
+++ b/python/Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisazaher/Documents/UNIVERSITY/4TH YR/ECE496 - Capstone/githubrepo/crapstone/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376F5AF4-9E36-6B4B-B73C-C6D04B51109F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5937476A-0D06-1B42-A2E1-89E844BAF45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15840" xr2:uid="{818555DF-D87D-7744-A63A-8FE4BECED375}"/>
   </bookViews>
@@ -573,7 +573,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -644,6 +644,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>